<commit_message>
Check number of distinct entrants in day rankings and all runs 2006-2009
</commit_message>
<xml_diff>
--- a/events/2008/rundata/2008.xlsx
+++ b/events/2008/rundata/2008.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\events\2008\rundata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0053B7-8EEE-4DBC-82F7-3AC483E8FBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FB572E-8A22-4AB6-9A27-AA4BAF8662F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{69F39C01-6DA0-46FD-BB01-BBC3FB8E10C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{69F39C01-6DA0-46FD-BB01-BBC3FB8E10C4}"/>
   </bookViews>
   <sheets>
     <sheet name="entrants" sheetId="8" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7815" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7816" uniqueCount="212">
   <si>
     <t>Sail Number</t>
   </si>
@@ -683,6 +683,9 @@
   <si>
     <t>?</t>
   </si>
+  <si>
+    <t>distinct</t>
+  </si>
 </sst>
 </file>
 
@@ -1052,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8024A034-A7EB-442D-A07F-57D7408A1B8A}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3017,11 +3020,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D33DF8-B7B4-4EB4-A626-3AADF234DB9A}">
-  <dimension ref="A1:H705"/>
+  <dimension ref="A1:H707"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A669" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A707" sqref="A707:B707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19252,6 +19255,15 @@
       </c>
       <c r="H705">
         <v>536</v>
+      </c>
+    </row>
+    <row r="707" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A707">
+        <f>SUMPRODUCT(1/COUNTIF(A$2:A705,A$2:A705))</f>
+        <v>77.000000000000327</v>
+      </c>
+      <c r="B707" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>